<commit_message>
date time zone ok
</commit_message>
<xml_diff>
--- a/sumTotal.xlsx
+++ b/sumTotal.xlsx
@@ -28,10 +28,10 @@
     <t>Material Name</t>
   </si>
   <si>
-    <t>Total Actual</t>
+    <t>Total Set</t>
   </si>
   <si>
-    <t>Total Set</t>
+    <t>Total Actual</t>
   </si>
   <si>
     <t>Total Diff</t>
@@ -657,16 +657,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1028,18 +1022,18 @@
   <dimension ref="A1:AM6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="20" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.7142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.4285714285714" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.2857142857143" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.8571428571429" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.71428571428571" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.7142857142857" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.4285714285714" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.8571428571429" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.71428571428571" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="4" customWidth="1"/>
     <col min="8" max="8" width="3.57142857142857" customWidth="1"/>
     <col min="9" max="9" width="3.85714285714286" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
@@ -1075,233 +1069,233 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:39">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:39">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="11">
+      <c r="B2" s="5"/>
+      <c r="C2" s="9">
         <v>43119.2490393519</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:39">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
-      <c r="AM3" s="16"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:39">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:39">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G6"/>

</xml_diff>